<commit_message>
adding latest fiels for submission
</commit_message>
<xml_diff>
--- a/dataset/rf/ManyntreePerformance.xlsx
+++ b/dataset/rf/ManyntreePerformance.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgil\Documents\Masters\dissertation\code\dataset\rf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D8926A9C-A022-4DC0-8010-E88A51F0E819}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A1EC9C-D629-48AE-B1A2-DF6B3B131ED5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="performance_df_ntree300_st_row1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">performance_df_ntree300_st_row1!$B$2:$B$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">performance_df_ntree300_st_row1!$D$2:$D$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">performance_df_ntree300_st_row1!$B$2:$B$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">performance_df_ntree300_st_row1!$D$2:$D$7</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -70,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,9 +624,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.5553149606299214E-2"/>
+          <c:x val="0.11610870516185477"/>
           <c:y val="5.0925925925925923E-2"/>
-          <c:w val="0.82889370078740154"/>
+          <c:w val="0.7705603674540682"/>
           <c:h val="0.80521580635753864"/>
         </c:manualLayout>
       </c:layout>
@@ -848,12 +842,7 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -981,6 +970,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="343030976"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1000,8 +990,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16222397200349956"/>
-          <c:y val="5.1504082822980461E-2"/>
+          <c:x val="0.15944619422572179"/>
+          <c:y val="2.3726305045202681E-2"/>
           <c:w val="0.63666294838145232"/>
           <c:h val="7.8125546806649182E-2"/>
         </c:manualLayout>
@@ -1721,6 +1711,186 @@
             </a:rPr>
             <a:t>Number of Trees</a:t>
           </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.20694</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.03833</cdr:x>
+      <cdr:y>0.65278</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F85D6A5B-0B40-4987-A006-5B130839637D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-523875" y="1091565"/>
+          <a:ext cx="1223010" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Sharpe Ratio, inv</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.96167</cdr:x>
+      <cdr:y>0.38241</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.75463</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4DC764B-7A0A-40D8-8DA1-E260E39F9F02}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="5400000">
+          <a:off x="3973830" y="1471930"/>
+          <a:ext cx="1021080" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>MSE</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2024,11 +2194,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>